<commit_message>
minor foregrip fix again
</commit_message>
<xml_diff>
--- a/changes/foregrips.xlsx
+++ b/changes/foregrips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E114C76-E32F-403F-BCC2-12977CD166B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B023C743-3C68-4849-BFD6-D451CA2E3A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,7 +1316,7 @@
   <dimension ref="A1:S69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,13 +1559,13 @@
         <v>114</v>
       </c>
       <c r="C8" s="23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="23">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E8" s="23">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="F8" s="23">
         <v>-2</v>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="N8" s="23">
         <f t="shared" si="0"/>
-        <v>7.2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>